<commit_message>
fix some fomatting in import students
</commit_message>
<xml_diff>
--- a/admin/Import_Student_template.xlsx
+++ b/admin/Import_Student_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gradeassist\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65494B58-A744-4B75-BF02-8EF232F3D69F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EDE24E-7958-49B3-B357-EE8C6A7F8233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{2D8A0C77-C8F6-4FC5-ADA5-6E30C659071A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{2D8A0C77-C8F6-4FC5-ADA5-6E30C659071A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>Mothers Name</t>
   </si>
   <si>
-    <t>Email Adresss</t>
-  </si>
-  <si>
     <t>Guardian Details</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Fathers Details</t>
+  </si>
+  <si>
+    <t>Fathers Name</t>
   </si>
 </sst>
 </file>
@@ -136,10 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -161,9 +160,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +200,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -307,7 +306,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,7 +448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -459,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6421643B-9976-4749-B363-532DBFA5EA17}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:W1"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,37 +487,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -527,68 +526,68 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="S2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>15</v>
+      <c r="W2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="X2" s="1"/>
     </row>

</xml_diff>